<commit_message>
invite command add, fix 2
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,15 +410,18 @@
         <v>UserID</v>
       </c>
       <c r="C1" t="str">
+        <v>InviteID</v>
+      </c>
+      <c r="D1" t="str">
         <v>ФИО</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Кем_работает</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Компания</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>ИНН_компании</v>
       </c>
     </row>
@@ -429,22 +432,25 @@
       <c r="B2" t="str">
         <v>@ftx3d</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2">
+        <v>351029552</v>
+      </c>
+      <c r="D2" t="str">
         <v>Шанашбаев Тимур Ермекович</v>
       </c>
-      <c r="D2" t="str">
-        <v>Делаю этого бота, программист</v>
-      </c>
       <c r="E2" t="str">
-        <v>Жана Самал</v>
+        <v>11111111111</v>
       </c>
       <c r="F2" t="str">
-        <v>11</v>
+        <v>22222222222</v>
+      </c>
+      <c r="G2" t="str">
+        <v>111111111111</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>